<commit_message>
problem 1 cleaning data
</commit_message>
<xml_diff>
--- a/data_hw2/mrtrashwheel.xlsx
+++ b/data_hw2/mrtrashwheel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahbowlin/Documents/Data Science 1/p8105_hw2_hmb2161/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahbowlin/Documents/Biostats Sem 1/Data Science 1/Data Science/p8105_homework2_hmb2161/data_hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE5836A7-1FB0-3640-9353-643A70CC3B0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739745D2-3DEE-DF44-8E88-59E80D417D94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="27580" windowHeight="16240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="460" windowWidth="27580" windowHeight="16120" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mr. Trash Wheel" sheetId="3" r:id="rId1"/>
@@ -1859,7 +1859,7 @@
   <dimension ref="A1:O339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="G334" sqref="G334"/>
     </sheetView>
@@ -17352,7 +17352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
@@ -21678,7 +21678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>

</xml_diff>